<commit_message>
Updated tests to include an invalid email and multiple emails in one cell
</commit_message>
<xml_diff>
--- a/tests/test_data/resident_list_mock.xlsx
+++ b/tests/test_data/resident_list_mock.xlsx
@@ -83,13 +83,13 @@
     <t xml:space="preserve">A2</t>
   </si>
   <si>
-    <t xml:space="preserve">test2@test.test</t>
+    <t xml:space="preserve">test2@test.test / test3@test.test</t>
   </si>
   <si>
     <t xml:space="preserve">A3</t>
   </si>
   <si>
-    <t xml:space="preserve">test3@test.test</t>
+    <t xml:space="preserve">asd</t>
   </si>
   <si>
     <t xml:space="preserve">B1</t>
@@ -226,16 +226,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,149 +322,149 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="29.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>17</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="N5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="L6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -518,10 +514,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="46.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.89"/>
   </cols>
@@ -559,35 +555,35 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed ldif_parser to use a sorted set so that there cannot be duplicate values which is not valid ldif
</commit_message>
<xml_diff>
--- a/tests/test_data/resident_list_mock.xlsx
+++ b/tests/test_data/resident_list_mock.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Päävuokraukset" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t xml:space="preserve">Asunto</t>
   </si>
@@ -319,10 +319,10 @@
   </sheetPr>
   <dimension ref="A1:Q82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,10 +501,10 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,6 +563,9 @@
       <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">

</xml_diff>